<commit_message>
fMRI + practice versions
</commit_message>
<xml_diff>
--- a/TMT_fmri/TMTstop-A_1_merged.xlsx
+++ b/TMT_fmri/TMTstop-A_1_merged.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lunduniversityo365-my.sharepoint.com/personal/em5456ol-s_lu_se/Documents/Experiment paradigms/TMT_PsychoPY_new/TMT_fmri/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="528" documentId="13_ncr:1_{ED9D02F7-1230-44A2-A7DC-15FEAC8DD2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0B6C3A4-B142-4655-8009-1956A601E02C}"/>
+  <xr:revisionPtr revIDLastSave="680" documentId="13_ncr:1_{ED9D02F7-1230-44A2-A7DC-15FEAC8DD2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6137F3CD-E19D-4F18-A71F-6FE5B28CF182}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5484" yWindow="900" windowWidth="17280" windowHeight="9024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="461">
   <si>
     <t>StimFile</t>
   </si>
@@ -49,15 +49,6 @@
   </si>
   <si>
     <t>NumberLetter</t>
-  </si>
-  <si>
-    <t>['1']</t>
-  </si>
-  <si>
-    <t>['2']</t>
-  </si>
-  <si>
-    <t>['3']</t>
   </si>
   <si>
     <t>TMTstop-A_1_1.png</t>
@@ -1745,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C160" sqref="C160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1766,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1778,36 +1769,37 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="H1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="B2" t="str">
+        <f>"['"&amp;C2&amp;"']"</f>
+        <v>['1']</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1820,23 +1812,24 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B66" si="0">"['"&amp;C3&amp;"']"</f>
+        <v>['3']</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1849,23 +1842,24 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1878,23 +1872,24 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1907,23 +1902,24 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1936,23 +1932,24 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1965,23 +1962,24 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1994,23 +1992,24 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G9" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2023,23 +2022,24 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2052,23 +2052,24 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G11" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -2081,23 +2082,24 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>6</v>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2110,23 +2112,24 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>7</v>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G13" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2139,23 +2142,24 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2168,23 +2172,24 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>7</v>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G15" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -2197,23 +2202,24 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>5</v>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2226,23 +2232,24 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>7</v>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G17" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2255,23 +2262,24 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>6</v>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G18" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -2284,23 +2292,24 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>7</v>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2313,23 +2322,24 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>5</v>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G20" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2342,23 +2352,24 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>7</v>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -2371,23 +2382,24 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>5</v>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E22" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G22" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2400,23 +2412,24 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>7</v>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C23">
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G23" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2429,23 +2442,24 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>5</v>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F24" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G24" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H24">
         <v>1</v>
@@ -2458,23 +2472,24 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>6</v>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G25" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H25">
         <v>1</v>
@@ -2487,23 +2502,24 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>7</v>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F26" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G26" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H26">
         <v>1</v>
@@ -2514,45 +2530,46 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F27" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
-      <c r="B28" t="s">
-        <v>7</v>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G28" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H28">
         <v>2</v>
@@ -2565,23 +2582,24 @@
       <c r="A29">
         <v>2</v>
       </c>
-      <c r="B29" t="s">
-        <v>6</v>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E29" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F29" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G29" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H29">
         <v>2</v>
@@ -2594,23 +2612,24 @@
       <c r="A30">
         <v>3</v>
       </c>
-      <c r="B30" t="s">
-        <v>7</v>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E30" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G30" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H30">
         <v>2</v>
@@ -2623,23 +2642,24 @@
       <c r="A31">
         <v>4</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G31" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H31">
         <v>2</v>
@@ -2652,23 +2672,24 @@
       <c r="A32">
         <v>5</v>
       </c>
-      <c r="B32" t="s">
-        <v>6</v>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E32" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G32" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H32">
         <v>2</v>
@@ -2681,23 +2702,24 @@
       <c r="A33">
         <v>6</v>
       </c>
-      <c r="B33" t="s">
-        <v>7</v>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C33">
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G33" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H33">
         <v>2</v>
@@ -2710,23 +2732,24 @@
       <c r="A34">
         <v>7</v>
       </c>
-      <c r="B34" t="s">
-        <v>6</v>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E34" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F34" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G34" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H34">
         <v>2</v>
@@ -2739,23 +2762,24 @@
       <c r="A35">
         <v>8</v>
       </c>
-      <c r="B35" t="s">
-        <v>5</v>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E35" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F35" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G35" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -2768,23 +2792,24 @@
       <c r="A36">
         <v>9</v>
       </c>
-      <c r="B36" t="s">
-        <v>6</v>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E36" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F36" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G36" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -2797,23 +2822,24 @@
       <c r="A37">
         <v>10</v>
       </c>
-      <c r="B37" t="s">
-        <v>7</v>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E37" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F37" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G37" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H37">
         <v>2</v>
@@ -2826,23 +2852,24 @@
       <c r="A38">
         <v>11</v>
       </c>
-      <c r="B38" t="s">
-        <v>5</v>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F38" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G38" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H38">
         <v>2</v>
@@ -2855,23 +2882,24 @@
       <c r="A39">
         <v>12</v>
       </c>
-      <c r="B39" t="s">
-        <v>6</v>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C39">
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E39" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F39" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G39" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H39">
         <v>2</v>
@@ -2884,23 +2912,24 @@
       <c r="A40">
         <v>13</v>
       </c>
-      <c r="B40" t="s">
-        <v>7</v>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E40" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F40" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G40" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H40">
         <v>2</v>
@@ -2913,23 +2942,24 @@
       <c r="A41">
         <v>14</v>
       </c>
-      <c r="B41" t="s">
-        <v>5</v>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F41" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G41" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H41">
         <v>2</v>
@@ -2942,23 +2972,24 @@
       <c r="A42">
         <v>15</v>
       </c>
-      <c r="B42" t="s">
-        <v>7</v>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E42" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F42" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G42" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H42">
         <v>2</v>
@@ -2971,23 +3002,24 @@
       <c r="A43">
         <v>16</v>
       </c>
-      <c r="B43" t="s">
-        <v>5</v>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E43" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F43" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G43" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H43">
         <v>2</v>
@@ -3000,23 +3032,24 @@
       <c r="A44">
         <v>17</v>
       </c>
-      <c r="B44" t="s">
-        <v>6</v>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E44" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F44" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G44" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H44">
         <v>2</v>
@@ -3029,23 +3062,24 @@
       <c r="A45">
         <v>18</v>
       </c>
-      <c r="B45" t="s">
-        <v>5</v>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E45" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F45" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G45" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H45">
         <v>2</v>
@@ -3058,23 +3092,24 @@
       <c r="A46">
         <v>19</v>
       </c>
-      <c r="B46" t="s">
-        <v>7</v>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E46" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F46" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G46" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H46">
         <v>2</v>
@@ -3087,23 +3122,24 @@
       <c r="A47">
         <v>20</v>
       </c>
-      <c r="B47" t="s">
-        <v>5</v>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D47" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E47" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F47" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G47" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H47">
         <v>2</v>
@@ -3116,23 +3152,24 @@
       <c r="A48">
         <v>21</v>
       </c>
-      <c r="B48" t="s">
-        <v>6</v>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E48" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F48" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G48" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H48">
         <v>2</v>
@@ -3145,23 +3182,24 @@
       <c r="A49">
         <v>22</v>
       </c>
-      <c r="B49" t="s">
-        <v>5</v>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D49" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E49" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F49" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G49" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H49">
         <v>2</v>
@@ -3174,23 +3212,24 @@
       <c r="A50">
         <v>23</v>
       </c>
-      <c r="B50" t="s">
-        <v>6</v>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E50" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F50" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G50" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H50">
         <v>2</v>
@@ -3203,23 +3242,24 @@
       <c r="A51">
         <v>24</v>
       </c>
-      <c r="B51" t="s">
-        <v>5</v>
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C51">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E51" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F51" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G51" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H51">
         <v>2</v>
@@ -3232,23 +3272,24 @@
       <c r="A52">
         <v>25</v>
       </c>
-      <c r="B52" t="s">
-        <v>6</v>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E52" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F52" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G52" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H52">
         <v>2</v>
@@ -3259,45 +3300,46 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D53" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E53" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F53" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G53" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H53">
         <v>2</v>
       </c>
       <c r="I53" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1</v>
       </c>
-      <c r="B54" t="s">
-        <v>6</v>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E54" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F54" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G54" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H54">
         <v>3</v>
@@ -3310,23 +3352,24 @@
       <c r="A55">
         <v>2</v>
       </c>
-      <c r="B55" t="s">
-        <v>5</v>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E55" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F55" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G55" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H55">
         <v>3</v>
@@ -3339,23 +3382,24 @@
       <c r="A56">
         <v>3</v>
       </c>
-      <c r="B56" t="s">
-        <v>7</v>
+      <c r="B56" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D56" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E56" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F56" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G56" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H56">
         <v>3</v>
@@ -3368,23 +3412,24 @@
       <c r="A57">
         <v>4</v>
       </c>
-      <c r="B57" t="s">
-        <v>6</v>
+      <c r="B57" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C57">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E57" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F57" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G57" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H57">
         <v>3</v>
@@ -3397,23 +3442,24 @@
       <c r="A58">
         <v>5</v>
       </c>
-      <c r="B58" t="s">
-        <v>7</v>
+      <c r="B58" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C58">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E58" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F58" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G58" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H58">
         <v>3</v>
@@ -3426,23 +3472,24 @@
       <c r="A59">
         <v>6</v>
       </c>
-      <c r="B59" t="s">
-        <v>6</v>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E59" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F59" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G59" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H59">
         <v>3</v>
@@ -3455,23 +3502,24 @@
       <c r="A60">
         <v>7</v>
       </c>
-      <c r="B60" t="s">
-        <v>5</v>
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E60" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F60" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G60" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H60">
         <v>3</v>
@@ -3484,23 +3532,24 @@
       <c r="A61">
         <v>8</v>
       </c>
-      <c r="B61" t="s">
-        <v>6</v>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E61" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F61" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G61" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H61">
         <v>3</v>
@@ -3513,23 +3562,24 @@
       <c r="A62">
         <v>9</v>
       </c>
-      <c r="B62" t="s">
-        <v>7</v>
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C62">
         <v>3</v>
       </c>
       <c r="D62" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E62" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F62" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G62" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H62">
         <v>3</v>
@@ -3542,23 +3592,24 @@
       <c r="A63">
         <v>10</v>
       </c>
-      <c r="B63" t="s">
-        <v>6</v>
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C63">
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E63" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F63" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G63" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H63">
         <v>3</v>
@@ -3571,23 +3622,24 @@
       <c r="A64">
         <v>11</v>
       </c>
-      <c r="B64" t="s">
-        <v>7</v>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>['3']</v>
       </c>
       <c r="C64">
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E64" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F64" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="G64" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H64">
         <v>3</v>
@@ -3600,23 +3652,24 @@
       <c r="A65">
         <v>12</v>
       </c>
-      <c r="B65" t="s">
-        <v>6</v>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>['2']</v>
       </c>
       <c r="C65">
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E65" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F65" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G65" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H65">
         <v>3</v>
@@ -3629,23 +3682,24 @@
       <c r="A66">
         <v>13</v>
       </c>
-      <c r="B66" t="s">
-        <v>5</v>
+      <c r="B66" t="str">
+        <f t="shared" si="0"/>
+        <v>['1']</v>
       </c>
       <c r="C66">
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E66" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F66" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G66" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H66">
         <v>3</v>
@@ -3658,23 +3712,24 @@
       <c r="A67">
         <v>14</v>
       </c>
-      <c r="B67" t="s">
-        <v>6</v>
+      <c r="B67" t="str">
+        <f t="shared" ref="B67:B130" si="1">"['"&amp;C67&amp;"']"</f>
+        <v>['2']</v>
       </c>
       <c r="C67">
         <v>2</v>
       </c>
       <c r="D67" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E67" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F67" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G67" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H67">
         <v>3</v>
@@ -3687,23 +3742,24 @@
       <c r="A68">
         <v>15</v>
       </c>
-      <c r="B68" t="s">
-        <v>5</v>
+      <c r="B68" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E68" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F68" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G68" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H68">
         <v>3</v>
@@ -3716,23 +3772,24 @@
       <c r="A69">
         <v>16</v>
       </c>
-      <c r="B69" t="s">
-        <v>6</v>
+      <c r="B69" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C69">
         <v>2</v>
       </c>
       <c r="D69" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E69" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F69" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G69" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H69">
         <v>3</v>
@@ -3745,23 +3802,24 @@
       <c r="A70">
         <v>17</v>
       </c>
-      <c r="B70" t="s">
-        <v>7</v>
+      <c r="B70" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C70">
         <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E70" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F70" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G70" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H70">
         <v>3</v>
@@ -3774,23 +3832,24 @@
       <c r="A71">
         <v>18</v>
       </c>
-      <c r="B71" t="s">
-        <v>6</v>
+      <c r="B71" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C71">
         <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E71" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F71" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G71" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H71">
         <v>3</v>
@@ -3803,23 +3862,24 @@
       <c r="A72">
         <v>19</v>
       </c>
-      <c r="B72" t="s">
-        <v>5</v>
+      <c r="B72" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E72" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F72" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G72" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H72">
         <v>3</v>
@@ -3832,23 +3892,24 @@
       <c r="A73">
         <v>20</v>
       </c>
-      <c r="B73" t="s">
-        <v>6</v>
+      <c r="B73" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E73" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F73" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G73" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H73">
         <v>3</v>
@@ -3861,23 +3922,24 @@
       <c r="A74">
         <v>21</v>
       </c>
-      <c r="B74" t="s">
-        <v>7</v>
+      <c r="B74" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C74">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E74" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F74" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G74" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H74">
         <v>3</v>
@@ -3890,23 +3952,24 @@
       <c r="A75">
         <v>22</v>
       </c>
-      <c r="B75" t="s">
-        <v>5</v>
+      <c r="B75" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E75" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F75" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G75" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H75">
         <v>3</v>
@@ -3919,23 +3982,24 @@
       <c r="A76">
         <v>23</v>
       </c>
-      <c r="B76" t="s">
-        <v>7</v>
+      <c r="B76" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C76">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D76" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E76" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F76" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G76" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H76">
         <v>3</v>
@@ -3948,23 +4012,24 @@
       <c r="A77">
         <v>24</v>
       </c>
-      <c r="B77" t="s">
-        <v>5</v>
+      <c r="B77" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C77">
         <v>1</v>
       </c>
       <c r="D77" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E77" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="F77" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G77" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H77">
         <v>3</v>
@@ -3977,23 +4042,24 @@
       <c r="A78">
         <v>25</v>
       </c>
-      <c r="B78" t="s">
-        <v>7</v>
+      <c r="B78" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C78">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D78" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E78" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F78" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G78" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H78">
         <v>3</v>
@@ -4004,45 +4070,46 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D79" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E79" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F79" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G79" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H79">
         <v>3</v>
       </c>
       <c r="I79" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1</v>
       </c>
-      <c r="B80" t="s">
-        <v>7</v>
+      <c r="B80" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C80">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E80" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F80" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G80" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H80">
         <v>4</v>
@@ -4055,23 +4122,24 @@
       <c r="A81">
         <v>2</v>
       </c>
-      <c r="B81" t="s">
-        <v>5</v>
+      <c r="B81" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C81">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E81" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F81" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G81" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H81">
         <v>4</v>
@@ -4084,23 +4152,24 @@
       <c r="A82">
         <v>3</v>
       </c>
-      <c r="B82" t="s">
-        <v>7</v>
+      <c r="B82" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C82">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="E82" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F82" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G82" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H82">
         <v>4</v>
@@ -4113,23 +4182,24 @@
       <c r="A83">
         <v>4</v>
       </c>
-      <c r="B83" t="s">
-        <v>5</v>
+      <c r="B83" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E83" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="F83" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G83" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H83">
         <v>4</v>
@@ -4142,23 +4212,24 @@
       <c r="A84">
         <v>5</v>
       </c>
-      <c r="B84" t="s">
-        <v>6</v>
+      <c r="B84" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C84">
         <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E84" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F84" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G84" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H84">
         <v>4</v>
@@ -4171,23 +4242,24 @@
       <c r="A85">
         <v>6</v>
       </c>
-      <c r="B85" t="s">
-        <v>7</v>
+      <c r="B85" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C85">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E85" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F85" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G85" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H85">
         <v>4</v>
@@ -4200,23 +4272,24 @@
       <c r="A86">
         <v>7</v>
       </c>
-      <c r="B86" t="s">
-        <v>6</v>
+      <c r="B86" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C86">
         <v>2</v>
       </c>
       <c r="D86" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="E86" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F86" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G86" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H86">
         <v>4</v>
@@ -4229,23 +4302,24 @@
       <c r="A87">
         <v>8</v>
       </c>
-      <c r="B87" t="s">
-        <v>7</v>
+      <c r="B87" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C87">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="E87" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F87" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="G87" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H87">
         <v>4</v>
@@ -4258,23 +4332,24 @@
       <c r="A88">
         <v>9</v>
       </c>
-      <c r="B88" t="s">
-        <v>5</v>
+      <c r="B88" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C88">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E88" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F88" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G88" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H88">
         <v>4</v>
@@ -4287,23 +4362,24 @@
       <c r="A89">
         <v>10</v>
       </c>
-      <c r="B89" t="s">
-        <v>6</v>
+      <c r="B89" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C89">
         <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="E89" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F89" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G89" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H89">
         <v>4</v>
@@ -4316,23 +4392,24 @@
       <c r="A90">
         <v>11</v>
       </c>
-      <c r="B90" t="s">
-        <v>7</v>
+      <c r="B90" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C90">
         <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E90" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="F90" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G90" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H90">
         <v>4</v>
@@ -4345,23 +4422,24 @@
       <c r="A91">
         <v>12</v>
       </c>
-      <c r="B91" t="s">
-        <v>5</v>
+      <c r="B91" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C91">
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="E91" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="F91" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G91" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H91">
         <v>4</v>
@@ -4374,23 +4452,24 @@
       <c r="A92">
         <v>13</v>
       </c>
-      <c r="B92" t="s">
-        <v>6</v>
+      <c r="B92" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E92" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="F92" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G92" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H92">
         <v>4</v>
@@ -4403,23 +4482,24 @@
       <c r="A93">
         <v>14</v>
       </c>
-      <c r="B93" t="s">
-        <v>5</v>
+      <c r="B93" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C93">
         <v>1</v>
       </c>
       <c r="D93" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="E93" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F93" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G93" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H93">
         <v>4</v>
@@ -4432,23 +4512,24 @@
       <c r="A94">
         <v>15</v>
       </c>
-      <c r="B94" t="s">
-        <v>6</v>
+      <c r="B94" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C94">
         <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E94" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="F94" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G94" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H94">
         <v>4</v>
@@ -4461,23 +4542,24 @@
       <c r="A95">
         <v>16</v>
       </c>
-      <c r="B95" t="s">
-        <v>7</v>
+      <c r="B95" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C95">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E95" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="F95" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G95" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H95">
         <v>4</v>
@@ -4490,23 +4572,24 @@
       <c r="A96">
         <v>17</v>
       </c>
-      <c r="B96" t="s">
-        <v>5</v>
+      <c r="B96" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C96">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D96" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="E96" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F96" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G96" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H96">
         <v>4</v>
@@ -4519,23 +4602,24 @@
       <c r="A97">
         <v>18</v>
       </c>
-      <c r="B97" t="s">
-        <v>6</v>
+      <c r="B97" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C97">
         <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E97" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="F97" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G97" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H97">
         <v>4</v>
@@ -4548,23 +4632,24 @@
       <c r="A98">
         <v>19</v>
       </c>
-      <c r="B98" t="s">
-        <v>5</v>
+      <c r="B98" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D98" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E98" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="F98" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G98" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H98">
         <v>4</v>
@@ -4577,23 +4662,24 @@
       <c r="A99">
         <v>20</v>
       </c>
-      <c r="B99" t="s">
-        <v>7</v>
+      <c r="B99" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C99">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E99" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="F99" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G99" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H99">
         <v>4</v>
@@ -4606,23 +4692,24 @@
       <c r="A100">
         <v>21</v>
       </c>
-      <c r="B100" t="s">
-        <v>5</v>
+      <c r="B100" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C100">
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="E100" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F100" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G100" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H100">
         <v>4</v>
@@ -4635,23 +4722,24 @@
       <c r="A101">
         <v>22</v>
       </c>
-      <c r="B101" t="s">
-        <v>7</v>
+      <c r="B101" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C101">
         <v>3</v>
       </c>
       <c r="D101" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E101" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F101" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G101" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H101">
         <v>4</v>
@@ -4664,23 +4752,24 @@
       <c r="A102">
         <v>23</v>
       </c>
-      <c r="B102" t="s">
-        <v>6</v>
+      <c r="B102" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C102">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E102" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="F102" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G102" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H102">
         <v>4</v>
@@ -4693,23 +4782,24 @@
       <c r="A103">
         <v>24</v>
       </c>
-      <c r="B103" t="s">
-        <v>7</v>
+      <c r="B103" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C103">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E103" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="F103" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G103" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H103">
         <v>4</v>
@@ -4722,23 +4812,24 @@
       <c r="A104">
         <v>25</v>
       </c>
-      <c r="B104" t="s">
-        <v>6</v>
+      <c r="B104" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C104">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D104" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E104" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="F104" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G104" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H104">
         <v>4</v>
@@ -4749,45 +4840,46 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D105" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E105" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="F105" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="G105" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H105">
         <v>4</v>
       </c>
       <c r="I105" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>1</v>
       </c>
-      <c r="B106" t="s">
-        <v>6</v>
+      <c r="B106" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C106">
         <v>2</v>
       </c>
       <c r="D106" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E106" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F106" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G106" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H106">
         <v>5</v>
@@ -4800,23 +4892,24 @@
       <c r="A107">
         <v>2</v>
       </c>
-      <c r="B107" t="s">
-        <v>5</v>
+      <c r="B107" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C107">
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E107" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="F107" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G107" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H107">
         <v>5</v>
@@ -4829,23 +4922,24 @@
       <c r="A108">
         <v>3</v>
       </c>
-      <c r="B108" t="s">
-        <v>7</v>
+      <c r="B108" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C108">
         <v>3</v>
       </c>
       <c r="D108" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E108" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F108" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G108" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H108">
         <v>5</v>
@@ -4858,23 +4952,24 @@
       <c r="A109">
         <v>4</v>
       </c>
-      <c r="B109" t="s">
-        <v>6</v>
+      <c r="B109" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C109">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D109" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E109" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F109" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G109" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H109">
         <v>5</v>
@@ -4887,23 +4982,24 @@
       <c r="A110">
         <v>5</v>
       </c>
-      <c r="B110" t="s">
-        <v>7</v>
+      <c r="B110" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C110">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D110" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E110" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F110" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G110" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H110">
         <v>5</v>
@@ -4916,23 +5012,24 @@
       <c r="A111">
         <v>6</v>
       </c>
-      <c r="B111" t="s">
-        <v>5</v>
+      <c r="B111" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C111">
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E111" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F111" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G111" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H111">
         <v>5</v>
@@ -4945,23 +5042,24 @@
       <c r="A112">
         <v>7</v>
       </c>
-      <c r="B112" t="s">
-        <v>7</v>
+      <c r="B112" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C112">
         <v>3</v>
       </c>
       <c r="D112" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E112" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F112" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G112" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H112">
         <v>5</v>
@@ -4974,23 +5072,24 @@
       <c r="A113">
         <v>8</v>
       </c>
-      <c r="B113" t="s">
-        <v>6</v>
+      <c r="B113" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C113">
         <v>2</v>
       </c>
       <c r="D113" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E113" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="F113" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G113" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H113">
         <v>5</v>
@@ -5003,23 +5102,24 @@
       <c r="A114">
         <v>9</v>
       </c>
-      <c r="B114" t="s">
-        <v>5</v>
+      <c r="B114" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C114">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D114" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E114" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F114" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G114" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H114">
         <v>5</v>
@@ -5032,23 +5132,24 @@
       <c r="A115">
         <v>10</v>
       </c>
-      <c r="B115" t="s">
-        <v>7</v>
+      <c r="B115" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C115">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D115" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E115" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F115" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="G115" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H115">
         <v>5</v>
@@ -5061,23 +5162,24 @@
       <c r="A116">
         <v>11</v>
       </c>
-      <c r="B116" t="s">
-        <v>6</v>
+      <c r="B116" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C116">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D116" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E116" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F116" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="G116" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H116">
         <v>5</v>
@@ -5090,23 +5192,24 @@
       <c r="A117">
         <v>12</v>
       </c>
-      <c r="B117" t="s">
-        <v>7</v>
+      <c r="B117" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C117">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E117" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F117" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="G117" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H117">
         <v>5</v>
@@ -5119,23 +5222,24 @@
       <c r="A118">
         <v>13</v>
       </c>
-      <c r="B118" t="s">
-        <v>5</v>
+      <c r="B118" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C118">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E118" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="F118" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G118" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H118">
         <v>5</v>
@@ -5148,23 +5252,24 @@
       <c r="A119">
         <v>14</v>
       </c>
-      <c r="B119" t="s">
-        <v>7</v>
+      <c r="B119" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C119">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E119" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="F119" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="G119" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H119">
         <v>5</v>
@@ -5177,23 +5282,24 @@
       <c r="A120">
         <v>15</v>
       </c>
-      <c r="B120" t="s">
-        <v>5</v>
+      <c r="B120" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C120">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D120" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E120" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F120" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="G120" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H120">
         <v>5</v>
@@ -5206,23 +5312,24 @@
       <c r="A121">
         <v>16</v>
       </c>
-      <c r="B121" t="s">
-        <v>7</v>
+      <c r="B121" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C121">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E121" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="F121" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G121" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H121">
         <v>5</v>
@@ -5235,23 +5342,24 @@
       <c r="A122">
         <v>17</v>
       </c>
-      <c r="B122" t="s">
-        <v>6</v>
+      <c r="B122" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C122">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E122" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="F122" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="G122" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H122">
         <v>5</v>
@@ -5264,23 +5372,24 @@
       <c r="A123">
         <v>18</v>
       </c>
-      <c r="B123" t="s">
-        <v>5</v>
+      <c r="B123" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C123">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D123" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E123" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F123" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="G123" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H123">
         <v>5</v>
@@ -5293,23 +5402,24 @@
       <c r="A124">
         <v>19</v>
       </c>
-      <c r="B124" t="s">
-        <v>7</v>
+      <c r="B124" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C124">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D124" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E124" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F124" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="G124" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H124">
         <v>5</v>
@@ -5322,23 +5432,24 @@
       <c r="A125">
         <v>20</v>
       </c>
-      <c r="B125" t="s">
-        <v>5</v>
+      <c r="B125" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C125">
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E125" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="F125" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="G125" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H125">
         <v>5</v>
@@ -5351,23 +5462,24 @@
       <c r="A126">
         <v>21</v>
       </c>
-      <c r="B126" t="s">
-        <v>6</v>
+      <c r="B126" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C126">
         <v>2</v>
       </c>
       <c r="D126" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E126" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F126" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="G126" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H126">
         <v>5</v>
@@ -5380,23 +5492,24 @@
       <c r="A127">
         <v>22</v>
       </c>
-      <c r="B127" t="s">
-        <v>7</v>
+      <c r="B127" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C127">
         <v>3</v>
       </c>
       <c r="D127" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E127" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F127" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="G127" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H127">
         <v>5</v>
@@ -5409,23 +5522,24 @@
       <c r="A128">
         <v>23</v>
       </c>
-      <c r="B128" t="s">
-        <v>6</v>
+      <c r="B128" t="str">
+        <f t="shared" si="1"/>
+        <v>['2']</v>
       </c>
       <c r="C128">
         <v>2</v>
       </c>
       <c r="D128" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E128" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F128" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G128" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H128">
         <v>5</v>
@@ -5438,23 +5552,24 @@
       <c r="A129">
         <v>24</v>
       </c>
-      <c r="B129" t="s">
-        <v>7</v>
+      <c r="B129" t="str">
+        <f t="shared" si="1"/>
+        <v>['3']</v>
       </c>
       <c r="C129">
         <v>3</v>
       </c>
       <c r="D129" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E129" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="F129" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="G129" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H129">
         <v>5</v>
@@ -5467,23 +5582,24 @@
       <c r="A130">
         <v>25</v>
       </c>
-      <c r="B130" t="s">
-        <v>6</v>
+      <c r="B130" t="str">
+        <f t="shared" si="1"/>
+        <v>['1']</v>
       </c>
       <c r="C130">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="E130" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="F130" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="G130" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H130">
         <v>5</v>
@@ -5494,45 +5610,46 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D131" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E131" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F131" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="G131" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H131">
         <v>5</v>
       </c>
       <c r="I131" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>1</v>
       </c>
-      <c r="B132" t="s">
-        <v>5</v>
+      <c r="B132" t="str">
+        <f t="shared" ref="B131:B156" si="2">"['"&amp;C132&amp;"']"</f>
+        <v>['3']</v>
       </c>
       <c r="C132">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D132" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E132" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F132" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="G132" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H132">
         <v>6</v>
@@ -5545,23 +5662,24 @@
       <c r="A133">
         <v>2</v>
       </c>
-      <c r="B133" t="s">
-        <v>6</v>
+      <c r="B133" t="str">
+        <f t="shared" si="2"/>
+        <v>['1']</v>
       </c>
       <c r="C133">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="E133" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F133" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G133" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H133">
         <v>6</v>
@@ -5574,23 +5692,24 @@
       <c r="A134">
         <v>3</v>
       </c>
-      <c r="B134" t="s">
-        <v>7</v>
+      <c r="B134" t="str">
+        <f t="shared" si="2"/>
+        <v>['2']</v>
       </c>
       <c r="C134">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D134" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E134" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F134" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G134" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H134">
         <v>6</v>
@@ -5603,23 +5722,24 @@
       <c r="A135">
         <v>4</v>
       </c>
-      <c r="B135" t="s">
-        <v>5</v>
+      <c r="B135" t="str">
+        <f t="shared" si="2"/>
+        <v>['1']</v>
       </c>
       <c r="C135">
         <v>1</v>
       </c>
       <c r="D135" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E135" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="F135" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G135" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H135">
         <v>6</v>
@@ -5632,23 +5752,24 @@
       <c r="A136">
         <v>5</v>
       </c>
-      <c r="B136" t="s">
-        <v>7</v>
+      <c r="B136" t="str">
+        <f t="shared" si="2"/>
+        <v>['2']</v>
       </c>
       <c r="C136">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D136" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="E136" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="F136" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G136" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H136">
         <v>6</v>
@@ -5661,23 +5782,24 @@
       <c r="A137">
         <v>6</v>
       </c>
-      <c r="B137" t="s">
-        <v>5</v>
+      <c r="B137" t="str">
+        <f t="shared" si="2"/>
+        <v>['3']</v>
       </c>
       <c r="C137">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D137" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="E137" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F137" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G137" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H137">
         <v>6</v>
@@ -5690,23 +5812,24 @@
       <c r="A138">
         <v>7</v>
       </c>
-      <c r="B138" t="s">
-        <v>7</v>
+      <c r="B138" t="str">
+        <f t="shared" si="2"/>
+        <v>['2']</v>
       </c>
       <c r="C138">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D138" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="E138" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F138" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G138" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H138">
         <v>6</v>
@@ -5719,23 +5842,24 @@
       <c r="A139">
         <v>8</v>
       </c>
-      <c r="B139" t="s">
-        <v>5</v>
+      <c r="B139" t="str">
+        <f t="shared" si="2"/>
+        <v>['1']</v>
       </c>
       <c r="C139">
         <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="E139" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="F139" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="G139" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H139">
         <v>6</v>
@@ -5748,23 +5872,24 @@
       <c r="A140">
         <v>9</v>
       </c>
-      <c r="B140" t="s">
-        <v>6</v>
+      <c r="B140" t="str">
+        <f t="shared" si="2"/>
+        <v>['3']</v>
       </c>
       <c r="C140">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D140" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="E140" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="F140" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="G140" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H140">
         <v>6</v>
@@ -5777,23 +5902,24 @@
       <c r="A141">
         <v>10</v>
       </c>
-      <c r="B141" t="s">
-        <v>7</v>
+      <c r="B141" t="str">
+        <f t="shared" si="2"/>
+        <v>['1']</v>
       </c>
       <c r="C141">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D141" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="E141" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="F141" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G141" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H141">
         <v>6</v>
@@ -5806,23 +5932,24 @@
       <c r="A142">
         <v>11</v>
       </c>
-      <c r="B142" t="s">
-        <v>5</v>
+      <c r="B142" t="str">
+        <f t="shared" si="2"/>
+        <v>['3']</v>
       </c>
       <c r="C142">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D142" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="E142" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F142" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G142" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H142">
         <v>6</v>
@@ -5835,23 +5962,24 @@
       <c r="A143">
         <v>12</v>
       </c>
-      <c r="B143" t="s">
-        <v>7</v>
+      <c r="B143" t="str">
+        <f t="shared" si="2"/>
+        <v>['2']</v>
       </c>
       <c r="C143">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D143" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="E143" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="F143" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="G143" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H143">
         <v>6</v>
@@ -5864,23 +5992,24 @@
       <c r="A144">
         <v>13</v>
       </c>
-      <c r="B144" t="s">
-        <v>6</v>
+      <c r="B144" t="str">
+        <f t="shared" si="2"/>
+        <v>['3']</v>
       </c>
       <c r="C144">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D144" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="E144" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="F144" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="G144" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H144">
         <v>6</v>
@@ -5893,23 +6022,24 @@
       <c r="A145">
         <v>14</v>
       </c>
-      <c r="B145" t="s">
-        <v>7</v>
+      <c r="B145" t="str">
+        <f t="shared" si="2"/>
+        <v>['1']</v>
       </c>
       <c r="C145">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E145" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="F145" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="G145" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H145">
         <v>6</v>
@@ -5922,23 +6052,24 @@
       <c r="A146">
         <v>15</v>
       </c>
-      <c r="B146" t="s">
-        <v>6</v>
+      <c r="B146" t="str">
+        <f t="shared" si="2"/>
+        <v>['3']</v>
       </c>
       <c r="C146">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D146" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="E146" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="F146" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G146" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H146">
         <v>6</v>
@@ -5951,23 +6082,24 @@
       <c r="A147">
         <v>16</v>
       </c>
-      <c r="B147" t="s">
-        <v>5</v>
+      <c r="B147" t="str">
+        <f t="shared" si="2"/>
+        <v>['1']</v>
       </c>
       <c r="C147">
         <v>1</v>
       </c>
       <c r="D147" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="E147" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="F147" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G147" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H147">
         <v>6</v>
@@ -5980,23 +6112,24 @@
       <c r="A148">
         <v>17</v>
       </c>
-      <c r="B148" t="s">
-        <v>7</v>
+      <c r="B148" t="str">
+        <f t="shared" si="2"/>
+        <v>['3']</v>
       </c>
       <c r="C148">
         <v>3</v>
       </c>
       <c r="D148" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="E148" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="F148" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="G148" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H148">
         <v>6</v>
@@ -6009,23 +6142,24 @@
       <c r="A149">
         <v>18</v>
       </c>
-      <c r="B149" t="s">
-        <v>5</v>
+      <c r="B149" t="str">
+        <f t="shared" si="2"/>
+        <v>['2']</v>
       </c>
       <c r="C149">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D149" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="E149" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="F149" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="G149" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H149">
         <v>6</v>
@@ -6038,23 +6172,24 @@
       <c r="A150">
         <v>19</v>
       </c>
-      <c r="B150" t="s">
-        <v>6</v>
+      <c r="B150" t="str">
+        <f t="shared" si="2"/>
+        <v>['3']</v>
       </c>
       <c r="C150">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D150" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="E150" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="F150" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="G150" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H150">
         <v>6</v>
@@ -6067,23 +6202,24 @@
       <c r="A151">
         <v>20</v>
       </c>
-      <c r="B151" t="s">
-        <v>7</v>
+      <c r="B151" t="str">
+        <f t="shared" si="2"/>
+        <v>['1']</v>
       </c>
       <c r="C151">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D151" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="E151" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="F151" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G151" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H151">
         <v>6</v>
@@ -6096,23 +6232,24 @@
       <c r="A152">
         <v>21</v>
       </c>
-      <c r="B152" t="s">
-        <v>6</v>
+      <c r="B152" t="str">
+        <f t="shared" si="2"/>
+        <v>['2']</v>
       </c>
       <c r="C152">
         <v>2</v>
       </c>
       <c r="D152" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="E152" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="F152" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G152" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H152">
         <v>6</v>
@@ -6125,23 +6262,24 @@
       <c r="A153">
         <v>22</v>
       </c>
-      <c r="B153" t="s">
-        <v>7</v>
+      <c r="B153" t="str">
+        <f t="shared" si="2"/>
+        <v>['1']</v>
       </c>
       <c r="C153">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="E153" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="F153" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="G153" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H153">
         <v>6</v>
@@ -6154,23 +6292,24 @@
       <c r="A154">
         <v>23</v>
       </c>
-      <c r="B154" t="s">
-        <v>5</v>
+      <c r="B154" t="str">
+        <f t="shared" si="2"/>
+        <v>['2']</v>
       </c>
       <c r="C154">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D154" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="E154" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="F154" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="G154" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H154">
         <v>6</v>
@@ -6183,23 +6322,24 @@
       <c r="A155">
         <v>24</v>
       </c>
-      <c r="B155" t="s">
-        <v>6</v>
+      <c r="B155" t="str">
+        <f t="shared" si="2"/>
+        <v>['3']</v>
       </c>
       <c r="C155">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D155" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="E155" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="F155" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="G155" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H155">
         <v>6</v>
@@ -6212,23 +6352,24 @@
       <c r="A156">
         <v>25</v>
       </c>
-      <c r="B156" t="s">
-        <v>7</v>
+      <c r="B156" t="str">
+        <f t="shared" si="2"/>
+        <v>['2']</v>
       </c>
       <c r="C156">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D156" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E156" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="F156" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="G156" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H156">
         <v>6</v>
@@ -6239,22 +6380,22 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D157" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="E157" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="F157" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="G157" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="H157">
         <v>6</v>
       </c>
       <c r="I157" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>